<commit_message>
add starz top ##
</commit_message>
<xml_diff>
--- a/create_defaults/template.xlsx
+++ b/create_defaults/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\TEST\create_defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2211EF27-D86F-4CCA-B115-AC184CA8CAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6532E39F-4817-4F28-91C2-CA48D08AB69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1275" windowWidth="19980" windowHeight="8850" xr2:uid="{C0516283-7CFC-4E92-8F0B-F8DC43661E92}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{C0516283-7CFC-4E92-8F0B-F8DC43661E92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11655" uniqueCount="2377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11865" uniqueCount="2379">
   <si>
     <t>key_name</t>
   </si>
@@ -7178,6 +7178,12 @@
   </si>
   <si>
     <t>#405162</t>
+  </si>
+  <si>
+    <t>Starz.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #464646</t>
   </si>
 </sst>
 </file>
@@ -7297,9 +7303,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7337,7 +7343,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7443,7 +7449,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7585,7 +7591,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7593,10 +7599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185220E8-1934-454F-B9D7-C7470B861D27}">
-  <dimension ref="A1:S802"/>
+  <dimension ref="A1:S832"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J781" workbookViewId="0">
-      <selection activeCell="M791" sqref="M791"/>
+    <sheetView tabSelected="1" topLeftCell="S774" workbookViewId="0">
+      <selection activeCell="S809" sqref="S780:S809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50245,17 +50251,20 @@
       </c>
     </row>
     <row r="780" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>2294</v>
+      </c>
       <c r="B780" t="s">
-        <v>2337</v>
+        <v>2377</v>
       </c>
       <c r="C780">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D780">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E780">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F780" t="s">
         <v>18</v>
@@ -50273,8 +50282,11 @@
         <v>19</v>
       </c>
       <c r="M780" t="str">
-        <f>SUBSTITUTE(B780,".png","")</f>
-        <v>Bleecker Street</v>
+        <f>"starz_" &amp; LOWER(A780)</f>
+        <v>starz_top_1</v>
+      </c>
+      <c r="N780" t="s">
+        <v>2378</v>
       </c>
       <c r="O780">
         <v>1</v>
@@ -50289,22 +50301,25 @@
         <v>1747</v>
       </c>
       <c r="S780" t="str">
-        <f t="shared" ref="S780:S802" si="31">"'"&amp;MID(A780,FIND(MID(TRIM(A780),1,1),A780),LEN(A780))&amp;"| "&amp;MID(B780,FIND(MID(TRIM(B780),1,1),B780),LEN(B780))&amp;"| +"&amp;C780&amp;"| "&amp;D780&amp;"| +"&amp;E780&amp;"| "&amp;MID(F780,FIND(MID(TRIM(F780),1,1),F780),LEN(F780))&amp;"| "&amp;G780&amp;"| "&amp;MID(H780,FIND(MID(TRIM(H780),1,1),H780),LEN(H780))&amp;"| "&amp;I780&amp;"| "&amp;J780&amp;"| "&amp;MID(K780,FIND(MID(TRIM(K780),1,1),K780),LEN(K780))&amp;"| "&amp;L780&amp;"| "&amp;MID(M780,FIND(MID(TRIM(M780),1,1),M780),LEN(M780))&amp;"| "&amp;MID(N780,FIND(MID(TRIM(N780),1,1),N780),LEN(N780))&amp;"| "&amp;MID(O780,FIND(MID(TRIM(O780),1,1),O780),LEN(O780))&amp;"| "&amp;MID(P780,FIND(MID(TRIM(P780),1,1),P780),LEN(P780))&amp;"| "&amp;MID(Q780,FIND(MID(TRIM(Q780),1,1),Q780),LEN(Q780))&amp;"| "&amp;MID(R780,FIND(MID(TRIM(R780),1,1),R780),LEN(R780))</f>
-        <v>'| Bleecker Street.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Bleecker Street| | 1| 1| 0| 1',</v>
+        <f t="shared" ref="S780:S809" si="31">"'"&amp;MID(A780,FIND(MID(TRIM(A780),1,1),A780),LEN(A780))&amp;"| "&amp;MID(B780,FIND(MID(TRIM(B780),1,1),B780),LEN(B780))&amp;"| +"&amp;C780&amp;"| "&amp;D780&amp;"| +"&amp;E780&amp;"| "&amp;MID(F780,FIND(MID(TRIM(F780),1,1),F780),LEN(F780))&amp;"| "&amp;G780&amp;"| "&amp;MID(H780,FIND(MID(TRIM(H780),1,1),H780),LEN(H780))&amp;"| "&amp;I780&amp;"| "&amp;J780&amp;"| "&amp;MID(K780,FIND(MID(TRIM(K780),1,1),K780),LEN(K780))&amp;"| "&amp;L780&amp;"| "&amp;MID(M780,FIND(MID(TRIM(M780),1,1),M780),LEN(M780))&amp;"| "&amp;MID(N780,FIND(MID(TRIM(N780),1,1),N780),LEN(N780))&amp;"| "&amp;MID(O780,FIND(MID(TRIM(O780),1,1),O780),LEN(O780))&amp;"| "&amp;MID(P780,FIND(MID(TRIM(P780),1,1),P780),LEN(P780))&amp;"| "&amp;MID(Q780,FIND(MID(TRIM(Q780),1,1),Q780),LEN(Q780))&amp;"| "&amp;MID(R780,FIND(MID(TRIM(R780),1,1),R780),LEN(R780))</f>
+        <v>'TOP_1| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_1| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="781" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>2308</v>
+      </c>
       <c r="B781" t="s">
-        <v>2338</v>
+        <v>2377</v>
       </c>
       <c r="C781">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D781">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E781">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F781" t="s">
         <v>18</v>
@@ -50322,8 +50337,11 @@
         <v>19</v>
       </c>
       <c r="M781" t="str">
-        <f t="shared" ref="M781:M786" si="32">SUBSTITUTE(B781,".png","")</f>
-        <v>IFC Films</v>
+        <f t="shared" ref="M781:M809" si="32">"starz_" &amp; LOWER(A781)</f>
+        <v>starz_top_2</v>
+      </c>
+      <c r="N781" t="s">
+        <v>2378</v>
       </c>
       <c r="O781">
         <v>1</v>
@@ -50339,21 +50357,24 @@
       </c>
       <c r="S781" t="str">
         <f t="shared" si="31"/>
-        <v>'| IFC Films.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | IFC Films| | 1| 1| 0| 1',</v>
+        <v>'TOP_2| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_2| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="782" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A782" t="s">
+        <v>2309</v>
+      </c>
       <c r="B782" t="s">
-        <v>2339</v>
+        <v>2377</v>
       </c>
       <c r="C782">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D782">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E782">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F782" t="s">
         <v>18</v>
@@ -50372,7 +50393,10 @@
       </c>
       <c r="M782" t="str">
         <f t="shared" si="32"/>
-        <v>NEON</v>
+        <v>starz_top_3</v>
+      </c>
+      <c r="N782" t="s">
+        <v>2378</v>
       </c>
       <c r="O782">
         <v>1</v>
@@ -50388,21 +50412,24 @@
       </c>
       <c r="S782" t="str">
         <f t="shared" si="31"/>
-        <v>'| NEON.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | NEON| | 1| 1| 0| 1',</v>
+        <v>'TOP_3| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_3| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="783" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A783" t="s">
+        <v>2310</v>
+      </c>
       <c r="B783" t="s">
-        <v>2340</v>
+        <v>2377</v>
       </c>
       <c r="C783">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D783">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E783">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F783" t="s">
         <v>18</v>
@@ -50421,7 +50448,10 @@
       </c>
       <c r="M783" t="str">
         <f t="shared" si="32"/>
-        <v>Rankin-Bass Productions</v>
+        <v>starz_top_4</v>
+      </c>
+      <c r="N783" t="s">
+        <v>2378</v>
       </c>
       <c r="O783">
         <v>1</v>
@@ -50437,21 +50467,24 @@
       </c>
       <c r="S783" t="str">
         <f t="shared" si="31"/>
-        <v>'| Rankin-Bass Productions.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Rankin-Bass Productions| | 1| 1| 0| 1',</v>
+        <v>'TOP_4| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_4| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="784" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A784" t="s">
+        <v>2311</v>
+      </c>
       <c r="B784" t="s">
-        <v>2341</v>
+        <v>2377</v>
       </c>
       <c r="C784">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D784">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E784">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F784" t="s">
         <v>18</v>
@@ -50470,7 +50503,10 @@
       </c>
       <c r="M784" t="str">
         <f t="shared" si="32"/>
-        <v>STX Entertainment</v>
+        <v>starz_top_5</v>
+      </c>
+      <c r="N784" t="s">
+        <v>2378</v>
       </c>
       <c r="O784">
         <v>1</v>
@@ -50486,21 +50522,24 @@
       </c>
       <c r="S784" t="str">
         <f t="shared" si="31"/>
-        <v>'| STX Entertainment.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | STX Entertainment| | 1| 1| 0| 1',</v>
+        <v>'TOP_5| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_5| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="785" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A785" t="s">
+        <v>2312</v>
+      </c>
       <c r="B785" t="s">
-        <v>2342</v>
+        <v>2377</v>
       </c>
       <c r="C785">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D785">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E785">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F785" t="s">
         <v>18</v>
@@ -50519,7 +50558,10 @@
       </c>
       <c r="M785" t="str">
         <f t="shared" si="32"/>
-        <v>TOHO</v>
+        <v>starz_top_6</v>
+      </c>
+      <c r="N785" t="s">
+        <v>2378</v>
       </c>
       <c r="O785">
         <v>1</v>
@@ -50535,21 +50577,24 @@
       </c>
       <c r="S785" t="str">
         <f t="shared" si="31"/>
-        <v>'| TOHO.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | TOHO| | 1| 1| 0| 1',</v>
+        <v>'TOP_6| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_6| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="786" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>2313</v>
+      </c>
       <c r="B786" t="s">
-        <v>2343</v>
+        <v>2377</v>
       </c>
       <c r="C786">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="D786">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="E786">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="F786" t="s">
         <v>18</v>
@@ -50568,7 +50613,10 @@
       </c>
       <c r="M786" t="str">
         <f t="shared" si="32"/>
-        <v>TSG Entertainment</v>
+        <v>starz_top_7</v>
+      </c>
+      <c r="N786" t="s">
+        <v>2378</v>
       </c>
       <c r="O786">
         <v>1</v>
@@ -50584,15 +50632,15 @@
       </c>
       <c r="S786" t="str">
         <f t="shared" si="31"/>
-        <v>'| TSG Entertainment.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | TSG Entertainment| | 1| 1| 0| 1',</v>
+        <v>'TOP_7| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_7| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="787" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>2344</v>
+        <v>2314</v>
       </c>
       <c r="B787" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C787">
         <v>-500</v>
@@ -50618,11 +50666,12 @@
       <c r="K787" t="s">
         <v>19</v>
       </c>
-      <c r="M787" t="s">
-        <v>2360</v>
+      <c r="M787" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_8</v>
       </c>
       <c r="N787" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O787">
         <v>1</v>
@@ -50634,19 +50683,19 @@
         <v>0</v>
       </c>
       <c r="R787" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S787" t="str">
         <f t="shared" si="31"/>
-        <v>'LETTERBOXD_TOP_250| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Letterboxd Top 250| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_8| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_8| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="788" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>2345</v>
+        <v>2315</v>
       </c>
       <c r="B788" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C788">
         <v>-500</v>
@@ -50672,11 +50721,12 @@
       <c r="K788" t="s">
         <v>19</v>
       </c>
-      <c r="M788" t="s">
-        <v>2361</v>
+      <c r="M788" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_9</v>
       </c>
       <c r="N788" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O788">
         <v>1</v>
@@ -50688,19 +50738,19 @@
         <v>0</v>
       </c>
       <c r="R788" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S788" t="str">
         <f t="shared" si="31"/>
-        <v>'BOX_OFFICE_MOJO_ALL_TIME_100| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Box Office Mojo All Time 100| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_9| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_9| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="789" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>2346</v>
+        <v>2336</v>
       </c>
       <c r="B789" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C789">
         <v>-500</v>
@@ -50726,11 +50776,12 @@
       <c r="K789" t="s">
         <v>19</v>
       </c>
-      <c r="M789" t="s">
-        <v>2362</v>
+      <c r="M789" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_10</v>
       </c>
       <c r="N789" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O789">
         <v>1</v>
@@ -50742,19 +50793,19 @@
         <v>0</v>
       </c>
       <c r="R789" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S789" t="str">
         <f t="shared" si="31"/>
-        <v>'AFI_100_YEARS_100_MOVIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | AFI 100 Years 100 Movies| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_10| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_10| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="790" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>2347</v>
+        <v>2316</v>
       </c>
       <c r="B790" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C790">
         <v>-500</v>
@@ -50780,11 +50831,12 @@
       <c r="K790" t="s">
         <v>19</v>
       </c>
-      <c r="M790" t="s">
-        <v>2363</v>
+      <c r="M790" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_11</v>
       </c>
       <c r="N790" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O790">
         <v>1</v>
@@ -50796,19 +50848,19 @@
         <v>0</v>
       </c>
       <c r="R790" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S790" t="str">
         <f t="shared" si="31"/>
-        <v>'SIGHT_AND_SOUND_GREATEST_FILMS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Sight &amp; Sound Greatest Films| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_11| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_11| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="791" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>1703</v>
+        <v>2317</v>
       </c>
       <c r="B791" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C791">
         <v>-500</v>
@@ -50834,11 +50886,12 @@
       <c r="K791" t="s">
         <v>19</v>
       </c>
-      <c r="M791" t="s">
-        <v>2375</v>
+      <c r="M791" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_12</v>
       </c>
       <c r="N791" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O791">
         <v>1</v>
@@ -50850,19 +50903,19 @@
         <v>0</v>
       </c>
       <c r="R791" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S791" t="str">
         <f t="shared" si="31"/>
-        <v>'1001_MOVIES_YOU_MUST_SEE_BEFORE_YOU_DIE| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | 1001 To See Before You Die| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_12| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_12| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="792" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>2348</v>
+        <v>2318</v>
       </c>
       <c r="B792" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C792">
         <v>-500</v>
@@ -50888,11 +50941,12 @@
       <c r="K792" t="s">
         <v>19</v>
       </c>
-      <c r="M792" t="s">
-        <v>2371</v>
+      <c r="M792" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_13</v>
       </c>
       <c r="N792" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O792">
         <v>1</v>
@@ -50904,19 +50958,19 @@
         <v>0</v>
       </c>
       <c r="R792" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S792" t="str">
         <f t="shared" si="31"/>
-        <v>'EDGAR_WRIGHTS_1000_FAVORITES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Edgar Wrights 1000 Favorites| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_13| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_13| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="793" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>2349</v>
+        <v>2319</v>
       </c>
       <c r="B793" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C793">
         <v>-500</v>
@@ -50942,11 +50996,12 @@
       <c r="K793" t="s">
         <v>19</v>
       </c>
-      <c r="M793" t="s">
-        <v>2372</v>
+      <c r="M793" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_14</v>
       </c>
       <c r="N793" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O793">
         <v>1</v>
@@ -50958,19 +51013,19 @@
         <v>0</v>
       </c>
       <c r="R793" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S793" t="str">
         <f t="shared" si="31"/>
-        <v>'ROGER_EBERTS_GREAT_MOVIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Roger Eberts Great Movies| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_14| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_14| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="794" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2350</v>
+        <v>2320</v>
       </c>
       <c r="B794" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C794">
         <v>-500</v>
@@ -50996,11 +51051,12 @@
       <c r="K794" t="s">
         <v>19</v>
       </c>
-      <c r="M794" t="s">
-        <v>2364</v>
+      <c r="M794" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_15</v>
       </c>
       <c r="N794" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O794">
         <v>1</v>
@@ -51012,19 +51068,19 @@
         <v>0</v>
       </c>
       <c r="R794" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S794" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_250_WOMEN_DIRECTED| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Women-Directed| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_15| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_15| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="795" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2351</v>
+        <v>2321</v>
       </c>
       <c r="B795" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C795">
         <v>-500</v>
@@ -51050,11 +51106,12 @@
       <c r="K795" t="s">
         <v>19</v>
       </c>
-      <c r="M795" t="s">
-        <v>2365</v>
+      <c r="M795" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_16</v>
       </c>
       <c r="N795" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O795">
         <v>1</v>
@@ -51066,19 +51123,19 @@
         <v>0</v>
       </c>
       <c r="R795" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S795" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_100_BLACK_DIRECTED| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 100 Black-Directed| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_16| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_16| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="796" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2352</v>
+        <v>2322</v>
       </c>
       <c r="B796" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C796">
         <v>-500</v>
@@ -51104,11 +51161,12 @@
       <c r="K796" t="s">
         <v>19</v>
       </c>
-      <c r="M796" t="s">
-        <v>2366</v>
+      <c r="M796" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_17</v>
       </c>
       <c r="N796" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O796">
         <v>1</v>
@@ -51120,19 +51178,19 @@
         <v>0</v>
       </c>
       <c r="R796" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S796" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_250_MOST_FANS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Most Fans| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_17| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_17| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="797" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2353</v>
+        <v>2323</v>
       </c>
       <c r="B797" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C797">
         <v>-500</v>
@@ -51158,11 +51216,12 @@
       <c r="K797" t="s">
         <v>19</v>
       </c>
-      <c r="M797" t="s">
-        <v>2367</v>
+      <c r="M797" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_18</v>
       </c>
       <c r="N797" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O797">
         <v>1</v>
@@ -51174,19 +51233,19 @@
         <v>0</v>
       </c>
       <c r="R797" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S797" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_250_DOCUMENTARIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Documentaries| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_18| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_18| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="798" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>2354</v>
+        <v>2324</v>
       </c>
       <c r="B798" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C798">
         <v>-500</v>
@@ -51212,11 +51271,12 @@
       <c r="K798" t="s">
         <v>19</v>
       </c>
-      <c r="M798" t="s">
-        <v>2368</v>
+      <c r="M798" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_19</v>
       </c>
       <c r="N798" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O798">
         <v>1</v>
@@ -51228,19 +51288,19 @@
         <v>0</v>
       </c>
       <c r="R798" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S798" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_100_ANIMATION| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 100 Animation| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_19| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_19| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="799" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>2355</v>
+        <v>2325</v>
       </c>
       <c r="B799" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C799">
         <v>-500</v>
@@ -51266,11 +51326,12 @@
       <c r="K799" t="s">
         <v>19</v>
       </c>
-      <c r="M799" t="s">
-        <v>2369</v>
+      <c r="M799" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_20</v>
       </c>
       <c r="N799" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O799">
         <v>1</v>
@@ -51282,19 +51343,19 @@
         <v>0</v>
       </c>
       <c r="R799" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S799" t="str">
         <f t="shared" si="31"/>
-        <v>'TOP_250_HORROR| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Horror| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_20| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_20| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="800" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>2356</v>
+        <v>2326</v>
       </c>
       <c r="B800" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C800">
         <v>-500</v>
@@ -51320,11 +51381,12 @@
       <c r="K800" t="s">
         <v>19</v>
       </c>
-      <c r="M800" t="s">
-        <v>2370</v>
+      <c r="M800" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_21</v>
       </c>
       <c r="N800" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O800">
         <v>1</v>
@@ -51336,19 +51398,19 @@
         <v>0</v>
       </c>
       <c r="R800" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S800" t="str">
         <f t="shared" si="31"/>
-        <v>'IMDB_TOP_250| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | IMDb Top 250| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_21| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_21| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="801" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>2357</v>
+        <v>2327</v>
       </c>
       <c r="B801" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C801">
         <v>-500</v>
@@ -51374,11 +51436,12 @@
       <c r="K801" t="s">
         <v>19</v>
       </c>
-      <c r="M801" t="s">
-        <v>2374</v>
+      <c r="M801" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_22</v>
       </c>
       <c r="N801" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O801">
         <v>1</v>
@@ -51390,19 +51453,19 @@
         <v>0</v>
       </c>
       <c r="R801" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S801" t="str">
         <f t="shared" si="31"/>
-        <v>'OSCARS_BEST_PICTURE_WINNERS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Oscars Best Picture Winners| #405162| 1| 1| 0| 0',</v>
+        <v>'TOP_22| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_22| #464646| 1| 1| 0| 1',</v>
       </c>
     </row>
     <row r="802" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>2358</v>
+        <v>2328</v>
       </c>
       <c r="B802" t="s">
-        <v>2359</v>
+        <v>2377</v>
       </c>
       <c r="C802">
         <v>-500</v>
@@ -51428,11 +51491,12 @@
       <c r="K802" t="s">
         <v>19</v>
       </c>
-      <c r="M802" t="s">
-        <v>2373</v>
+      <c r="M802" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_23</v>
       </c>
       <c r="N802" t="s">
-        <v>2376</v>
+        <v>2378</v>
       </c>
       <c r="O802">
         <v>1</v>
@@ -51444,10 +51508,1602 @@
         <v>0</v>
       </c>
       <c r="R802" t="s">
-        <v>20</v>
+        <v>1747</v>
       </c>
       <c r="S802" t="str">
         <f t="shared" si="31"/>
+        <v>'TOP_23| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_23| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="803" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A803" t="s">
+        <v>2329</v>
+      </c>
+      <c r="B803" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C803">
+        <v>-500</v>
+      </c>
+      <c r="D803">
+        <v>1500</v>
+      </c>
+      <c r="E803">
+        <v>850</v>
+      </c>
+      <c r="F803" t="s">
+        <v>18</v>
+      </c>
+      <c r="H803" t="s">
+        <v>19</v>
+      </c>
+      <c r="I803">
+        <v>0</v>
+      </c>
+      <c r="J803">
+        <v>15</v>
+      </c>
+      <c r="K803" t="s">
+        <v>19</v>
+      </c>
+      <c r="M803" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_24</v>
+      </c>
+      <c r="N803" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O803">
+        <v>1</v>
+      </c>
+      <c r="P803">
+        <v>1</v>
+      </c>
+      <c r="Q803">
+        <v>0</v>
+      </c>
+      <c r="R803" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S803" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_24| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_24| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="804" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A804" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B804" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C804">
+        <v>-500</v>
+      </c>
+      <c r="D804">
+        <v>1500</v>
+      </c>
+      <c r="E804">
+        <v>850</v>
+      </c>
+      <c r="F804" t="s">
+        <v>18</v>
+      </c>
+      <c r="H804" t="s">
+        <v>19</v>
+      </c>
+      <c r="I804">
+        <v>0</v>
+      </c>
+      <c r="J804">
+        <v>15</v>
+      </c>
+      <c r="K804" t="s">
+        <v>19</v>
+      </c>
+      <c r="M804" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_25</v>
+      </c>
+      <c r="N804" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O804">
+        <v>1</v>
+      </c>
+      <c r="P804">
+        <v>1</v>
+      </c>
+      <c r="Q804">
+        <v>0</v>
+      </c>
+      <c r="R804" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S804" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_25| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_25| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="805" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B805" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C805">
+        <v>-500</v>
+      </c>
+      <c r="D805">
+        <v>1500</v>
+      </c>
+      <c r="E805">
+        <v>850</v>
+      </c>
+      <c r="F805" t="s">
+        <v>18</v>
+      </c>
+      <c r="H805" t="s">
+        <v>19</v>
+      </c>
+      <c r="I805">
+        <v>0</v>
+      </c>
+      <c r="J805">
+        <v>15</v>
+      </c>
+      <c r="K805" t="s">
+        <v>19</v>
+      </c>
+      <c r="M805" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_26</v>
+      </c>
+      <c r="N805" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O805">
+        <v>1</v>
+      </c>
+      <c r="P805">
+        <v>1</v>
+      </c>
+      <c r="Q805">
+        <v>0</v>
+      </c>
+      <c r="R805" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S805" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_26| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_26| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="806" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A806" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B806" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C806">
+        <v>-500</v>
+      </c>
+      <c r="D806">
+        <v>1500</v>
+      </c>
+      <c r="E806">
+        <v>850</v>
+      </c>
+      <c r="F806" t="s">
+        <v>18</v>
+      </c>
+      <c r="H806" t="s">
+        <v>19</v>
+      </c>
+      <c r="I806">
+        <v>0</v>
+      </c>
+      <c r="J806">
+        <v>15</v>
+      </c>
+      <c r="K806" t="s">
+        <v>19</v>
+      </c>
+      <c r="M806" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_27</v>
+      </c>
+      <c r="N806" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O806">
+        <v>1</v>
+      </c>
+      <c r="P806">
+        <v>1</v>
+      </c>
+      <c r="Q806">
+        <v>0</v>
+      </c>
+      <c r="R806" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S806" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_27| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_27| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="807" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A807" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B807" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C807">
+        <v>-500</v>
+      </c>
+      <c r="D807">
+        <v>1500</v>
+      </c>
+      <c r="E807">
+        <v>850</v>
+      </c>
+      <c r="F807" t="s">
+        <v>18</v>
+      </c>
+      <c r="H807" t="s">
+        <v>19</v>
+      </c>
+      <c r="I807">
+        <v>0</v>
+      </c>
+      <c r="J807">
+        <v>15</v>
+      </c>
+      <c r="K807" t="s">
+        <v>19</v>
+      </c>
+      <c r="M807" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_28</v>
+      </c>
+      <c r="N807" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O807">
+        <v>1</v>
+      </c>
+      <c r="P807">
+        <v>1</v>
+      </c>
+      <c r="Q807">
+        <v>0</v>
+      </c>
+      <c r="R807" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S807" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_28| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_28| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="808" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A808" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B808" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C808">
+        <v>-500</v>
+      </c>
+      <c r="D808">
+        <v>1500</v>
+      </c>
+      <c r="E808">
+        <v>850</v>
+      </c>
+      <c r="F808" t="s">
+        <v>18</v>
+      </c>
+      <c r="H808" t="s">
+        <v>19</v>
+      </c>
+      <c r="I808">
+        <v>0</v>
+      </c>
+      <c r="J808">
+        <v>15</v>
+      </c>
+      <c r="K808" t="s">
+        <v>19</v>
+      </c>
+      <c r="M808" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_29</v>
+      </c>
+      <c r="N808" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O808">
+        <v>1</v>
+      </c>
+      <c r="P808">
+        <v>1</v>
+      </c>
+      <c r="Q808">
+        <v>0</v>
+      </c>
+      <c r="R808" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S808" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_29| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_29| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="809" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A809" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B809" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C809">
+        <v>-500</v>
+      </c>
+      <c r="D809">
+        <v>1500</v>
+      </c>
+      <c r="E809">
+        <v>850</v>
+      </c>
+      <c r="F809" t="s">
+        <v>18</v>
+      </c>
+      <c r="H809" t="s">
+        <v>19</v>
+      </c>
+      <c r="I809">
+        <v>0</v>
+      </c>
+      <c r="J809">
+        <v>15</v>
+      </c>
+      <c r="K809" t="s">
+        <v>19</v>
+      </c>
+      <c r="M809" t="str">
+        <f t="shared" si="32"/>
+        <v>starz_top_30</v>
+      </c>
+      <c r="N809" t="s">
+        <v>2378</v>
+      </c>
+      <c r="O809">
+        <v>1</v>
+      </c>
+      <c r="P809">
+        <v>1</v>
+      </c>
+      <c r="Q809">
+        <v>0</v>
+      </c>
+      <c r="R809" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S809" t="str">
+        <f t="shared" si="31"/>
+        <v>'TOP_30| Starz.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | starz_top_30| #464646| 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="810" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B810" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C810">
+        <v>0</v>
+      </c>
+      <c r="D810">
+        <v>1600</v>
+      </c>
+      <c r="E810">
+        <v>0</v>
+      </c>
+      <c r="F810" t="s">
+        <v>18</v>
+      </c>
+      <c r="H810" t="s">
+        <v>19</v>
+      </c>
+      <c r="I810">
+        <v>0</v>
+      </c>
+      <c r="J810">
+        <v>15</v>
+      </c>
+      <c r="K810" t="s">
+        <v>19</v>
+      </c>
+      <c r="M810" t="str">
+        <f>SUBSTITUTE(B810,".png","")</f>
+        <v>Bleecker Street</v>
+      </c>
+      <c r="O810">
+        <v>1</v>
+      </c>
+      <c r="P810">
+        <v>1</v>
+      </c>
+      <c r="Q810">
+        <v>0</v>
+      </c>
+      <c r="R810" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S810" t="str">
+        <f t="shared" ref="S810:S832" si="33">"'"&amp;MID(A810,FIND(MID(TRIM(A810),1,1),A810),LEN(A810))&amp;"| "&amp;MID(B810,FIND(MID(TRIM(B810),1,1),B810),LEN(B810))&amp;"| +"&amp;C810&amp;"| "&amp;D810&amp;"| +"&amp;E810&amp;"| "&amp;MID(F810,FIND(MID(TRIM(F810),1,1),F810),LEN(F810))&amp;"| "&amp;G810&amp;"| "&amp;MID(H810,FIND(MID(TRIM(H810),1,1),H810),LEN(H810))&amp;"| "&amp;I810&amp;"| "&amp;J810&amp;"| "&amp;MID(K810,FIND(MID(TRIM(K810),1,1),K810),LEN(K810))&amp;"| "&amp;L810&amp;"| "&amp;MID(M810,FIND(MID(TRIM(M810),1,1),M810),LEN(M810))&amp;"| "&amp;MID(N810,FIND(MID(TRIM(N810),1,1),N810),LEN(N810))&amp;"| "&amp;MID(O810,FIND(MID(TRIM(O810),1,1),O810),LEN(O810))&amp;"| "&amp;MID(P810,FIND(MID(TRIM(P810),1,1),P810),LEN(P810))&amp;"| "&amp;MID(Q810,FIND(MID(TRIM(Q810),1,1),Q810),LEN(Q810))&amp;"| "&amp;MID(R810,FIND(MID(TRIM(R810),1,1),R810),LEN(R810))</f>
+        <v>'| Bleecker Street.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Bleecker Street| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="811" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B811" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C811">
+        <v>0</v>
+      </c>
+      <c r="D811">
+        <v>1600</v>
+      </c>
+      <c r="E811">
+        <v>0</v>
+      </c>
+      <c r="F811" t="s">
+        <v>18</v>
+      </c>
+      <c r="H811" t="s">
+        <v>19</v>
+      </c>
+      <c r="I811">
+        <v>0</v>
+      </c>
+      <c r="J811">
+        <v>15</v>
+      </c>
+      <c r="K811" t="s">
+        <v>19</v>
+      </c>
+      <c r="M811" t="str">
+        <f t="shared" ref="M811:M816" si="34">SUBSTITUTE(B811,".png","")</f>
+        <v>IFC Films</v>
+      </c>
+      <c r="O811">
+        <v>1</v>
+      </c>
+      <c r="P811">
+        <v>1</v>
+      </c>
+      <c r="Q811">
+        <v>0</v>
+      </c>
+      <c r="R811" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S811" t="str">
+        <f t="shared" si="33"/>
+        <v>'| IFC Films.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | IFC Films| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="812" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B812" t="s">
+        <v>2339</v>
+      </c>
+      <c r="C812">
+        <v>0</v>
+      </c>
+      <c r="D812">
+        <v>1600</v>
+      </c>
+      <c r="E812">
+        <v>0</v>
+      </c>
+      <c r="F812" t="s">
+        <v>18</v>
+      </c>
+      <c r="H812" t="s">
+        <v>19</v>
+      </c>
+      <c r="I812">
+        <v>0</v>
+      </c>
+      <c r="J812">
+        <v>15</v>
+      </c>
+      <c r="K812" t="s">
+        <v>19</v>
+      </c>
+      <c r="M812" t="str">
+        <f t="shared" si="34"/>
+        <v>NEON</v>
+      </c>
+      <c r="O812">
+        <v>1</v>
+      </c>
+      <c r="P812">
+        <v>1</v>
+      </c>
+      <c r="Q812">
+        <v>0</v>
+      </c>
+      <c r="R812" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S812" t="str">
+        <f t="shared" si="33"/>
+        <v>'| NEON.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | NEON| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="813" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B813" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C813">
+        <v>0</v>
+      </c>
+      <c r="D813">
+        <v>1600</v>
+      </c>
+      <c r="E813">
+        <v>0</v>
+      </c>
+      <c r="F813" t="s">
+        <v>18</v>
+      </c>
+      <c r="H813" t="s">
+        <v>19</v>
+      </c>
+      <c r="I813">
+        <v>0</v>
+      </c>
+      <c r="J813">
+        <v>15</v>
+      </c>
+      <c r="K813" t="s">
+        <v>19</v>
+      </c>
+      <c r="M813" t="str">
+        <f t="shared" si="34"/>
+        <v>Rankin-Bass Productions</v>
+      </c>
+      <c r="O813">
+        <v>1</v>
+      </c>
+      <c r="P813">
+        <v>1</v>
+      </c>
+      <c r="Q813">
+        <v>0</v>
+      </c>
+      <c r="R813" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S813" t="str">
+        <f t="shared" si="33"/>
+        <v>'| Rankin-Bass Productions.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Rankin-Bass Productions| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="814" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B814" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C814">
+        <v>0</v>
+      </c>
+      <c r="D814">
+        <v>1600</v>
+      </c>
+      <c r="E814">
+        <v>0</v>
+      </c>
+      <c r="F814" t="s">
+        <v>18</v>
+      </c>
+      <c r="H814" t="s">
+        <v>19</v>
+      </c>
+      <c r="I814">
+        <v>0</v>
+      </c>
+      <c r="J814">
+        <v>15</v>
+      </c>
+      <c r="K814" t="s">
+        <v>19</v>
+      </c>
+      <c r="M814" t="str">
+        <f t="shared" si="34"/>
+        <v>STX Entertainment</v>
+      </c>
+      <c r="O814">
+        <v>1</v>
+      </c>
+      <c r="P814">
+        <v>1</v>
+      </c>
+      <c r="Q814">
+        <v>0</v>
+      </c>
+      <c r="R814" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S814" t="str">
+        <f t="shared" si="33"/>
+        <v>'| STX Entertainment.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | STX Entertainment| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="815" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B815" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C815">
+        <v>0</v>
+      </c>
+      <c r="D815">
+        <v>1600</v>
+      </c>
+      <c r="E815">
+        <v>0</v>
+      </c>
+      <c r="F815" t="s">
+        <v>18</v>
+      </c>
+      <c r="H815" t="s">
+        <v>19</v>
+      </c>
+      <c r="I815">
+        <v>0</v>
+      </c>
+      <c r="J815">
+        <v>15</v>
+      </c>
+      <c r="K815" t="s">
+        <v>19</v>
+      </c>
+      <c r="M815" t="str">
+        <f t="shared" si="34"/>
+        <v>TOHO</v>
+      </c>
+      <c r="O815">
+        <v>1</v>
+      </c>
+      <c r="P815">
+        <v>1</v>
+      </c>
+      <c r="Q815">
+        <v>0</v>
+      </c>
+      <c r="R815" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S815" t="str">
+        <f t="shared" si="33"/>
+        <v>'| TOHO.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | TOHO| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="816" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B816" t="s">
+        <v>2343</v>
+      </c>
+      <c r="C816">
+        <v>0</v>
+      </c>
+      <c r="D816">
+        <v>1600</v>
+      </c>
+      <c r="E816">
+        <v>0</v>
+      </c>
+      <c r="F816" t="s">
+        <v>18</v>
+      </c>
+      <c r="H816" t="s">
+        <v>19</v>
+      </c>
+      <c r="I816">
+        <v>0</v>
+      </c>
+      <c r="J816">
+        <v>15</v>
+      </c>
+      <c r="K816" t="s">
+        <v>19</v>
+      </c>
+      <c r="M816" t="str">
+        <f t="shared" si="34"/>
+        <v>TSG Entertainment</v>
+      </c>
+      <c r="O816">
+        <v>1</v>
+      </c>
+      <c r="P816">
+        <v>1</v>
+      </c>
+      <c r="Q816">
+        <v>0</v>
+      </c>
+      <c r="R816" t="s">
+        <v>1747</v>
+      </c>
+      <c r="S816" t="str">
+        <f t="shared" si="33"/>
+        <v>'| TSG Entertainment.png| +0| 1600| +0| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | TSG Entertainment| | 1| 1| 0| 1',</v>
+      </c>
+    </row>
+    <row r="817" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>2344</v>
+      </c>
+      <c r="B817" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C817">
+        <v>-500</v>
+      </c>
+      <c r="D817">
+        <v>1500</v>
+      </c>
+      <c r="E817">
+        <v>850</v>
+      </c>
+      <c r="F817" t="s">
+        <v>18</v>
+      </c>
+      <c r="H817" t="s">
+        <v>19</v>
+      </c>
+      <c r="I817">
+        <v>0</v>
+      </c>
+      <c r="J817">
+        <v>15</v>
+      </c>
+      <c r="K817" t="s">
+        <v>19</v>
+      </c>
+      <c r="M817" t="s">
+        <v>2360</v>
+      </c>
+      <c r="N817" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O817">
+        <v>1</v>
+      </c>
+      <c r="P817">
+        <v>1</v>
+      </c>
+      <c r="Q817">
+        <v>0</v>
+      </c>
+      <c r="R817" t="s">
+        <v>20</v>
+      </c>
+      <c r="S817" t="str">
+        <f t="shared" si="33"/>
+        <v>'LETTERBOXD_TOP_250| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Letterboxd Top 250| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="818" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B818" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C818">
+        <v>-500</v>
+      </c>
+      <c r="D818">
+        <v>1500</v>
+      </c>
+      <c r="E818">
+        <v>850</v>
+      </c>
+      <c r="F818" t="s">
+        <v>18</v>
+      </c>
+      <c r="H818" t="s">
+        <v>19</v>
+      </c>
+      <c r="I818">
+        <v>0</v>
+      </c>
+      <c r="J818">
+        <v>15</v>
+      </c>
+      <c r="K818" t="s">
+        <v>19</v>
+      </c>
+      <c r="M818" t="s">
+        <v>2361</v>
+      </c>
+      <c r="N818" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O818">
+        <v>1</v>
+      </c>
+      <c r="P818">
+        <v>1</v>
+      </c>
+      <c r="Q818">
+        <v>0</v>
+      </c>
+      <c r="R818" t="s">
+        <v>20</v>
+      </c>
+      <c r="S818" t="str">
+        <f t="shared" si="33"/>
+        <v>'BOX_OFFICE_MOJO_ALL_TIME_100| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Box Office Mojo All Time 100| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="819" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B819" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C819">
+        <v>-500</v>
+      </c>
+      <c r="D819">
+        <v>1500</v>
+      </c>
+      <c r="E819">
+        <v>850</v>
+      </c>
+      <c r="F819" t="s">
+        <v>18</v>
+      </c>
+      <c r="H819" t="s">
+        <v>19</v>
+      </c>
+      <c r="I819">
+        <v>0</v>
+      </c>
+      <c r="J819">
+        <v>15</v>
+      </c>
+      <c r="K819" t="s">
+        <v>19</v>
+      </c>
+      <c r="M819" t="s">
+        <v>2362</v>
+      </c>
+      <c r="N819" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O819">
+        <v>1</v>
+      </c>
+      <c r="P819">
+        <v>1</v>
+      </c>
+      <c r="Q819">
+        <v>0</v>
+      </c>
+      <c r="R819" t="s">
+        <v>20</v>
+      </c>
+      <c r="S819" t="str">
+        <f t="shared" si="33"/>
+        <v>'AFI_100_YEARS_100_MOVIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | AFI 100 Years 100 Movies| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="820" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B820" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C820">
+        <v>-500</v>
+      </c>
+      <c r="D820">
+        <v>1500</v>
+      </c>
+      <c r="E820">
+        <v>850</v>
+      </c>
+      <c r="F820" t="s">
+        <v>18</v>
+      </c>
+      <c r="H820" t="s">
+        <v>19</v>
+      </c>
+      <c r="I820">
+        <v>0</v>
+      </c>
+      <c r="J820">
+        <v>15</v>
+      </c>
+      <c r="K820" t="s">
+        <v>19</v>
+      </c>
+      <c r="M820" t="s">
+        <v>2363</v>
+      </c>
+      <c r="N820" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O820">
+        <v>1</v>
+      </c>
+      <c r="P820">
+        <v>1</v>
+      </c>
+      <c r="Q820">
+        <v>0</v>
+      </c>
+      <c r="R820" t="s">
+        <v>20</v>
+      </c>
+      <c r="S820" t="str">
+        <f t="shared" si="33"/>
+        <v>'SIGHT_AND_SOUND_GREATEST_FILMS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Sight &amp; Sound Greatest Films| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="821" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B821" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C821">
+        <v>-500</v>
+      </c>
+      <c r="D821">
+        <v>1500</v>
+      </c>
+      <c r="E821">
+        <v>850</v>
+      </c>
+      <c r="F821" t="s">
+        <v>18</v>
+      </c>
+      <c r="H821" t="s">
+        <v>19</v>
+      </c>
+      <c r="I821">
+        <v>0</v>
+      </c>
+      <c r="J821">
+        <v>15</v>
+      </c>
+      <c r="K821" t="s">
+        <v>19</v>
+      </c>
+      <c r="M821" t="s">
+        <v>2375</v>
+      </c>
+      <c r="N821" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O821">
+        <v>1</v>
+      </c>
+      <c r="P821">
+        <v>1</v>
+      </c>
+      <c r="Q821">
+        <v>0</v>
+      </c>
+      <c r="R821" t="s">
+        <v>20</v>
+      </c>
+      <c r="S821" t="str">
+        <f t="shared" si="33"/>
+        <v>'1001_MOVIES_YOU_MUST_SEE_BEFORE_YOU_DIE| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | 1001 To See Before You Die| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="822" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>2348</v>
+      </c>
+      <c r="B822" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C822">
+        <v>-500</v>
+      </c>
+      <c r="D822">
+        <v>1500</v>
+      </c>
+      <c r="E822">
+        <v>850</v>
+      </c>
+      <c r="F822" t="s">
+        <v>18</v>
+      </c>
+      <c r="H822" t="s">
+        <v>19</v>
+      </c>
+      <c r="I822">
+        <v>0</v>
+      </c>
+      <c r="J822">
+        <v>15</v>
+      </c>
+      <c r="K822" t="s">
+        <v>19</v>
+      </c>
+      <c r="M822" t="s">
+        <v>2371</v>
+      </c>
+      <c r="N822" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O822">
+        <v>1</v>
+      </c>
+      <c r="P822">
+        <v>1</v>
+      </c>
+      <c r="Q822">
+        <v>0</v>
+      </c>
+      <c r="R822" t="s">
+        <v>20</v>
+      </c>
+      <c r="S822" t="str">
+        <f t="shared" si="33"/>
+        <v>'EDGAR_WRIGHTS_1000_FAVORITES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Edgar Wrights 1000 Favorites| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="823" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B823" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C823">
+        <v>-500</v>
+      </c>
+      <c r="D823">
+        <v>1500</v>
+      </c>
+      <c r="E823">
+        <v>850</v>
+      </c>
+      <c r="F823" t="s">
+        <v>18</v>
+      </c>
+      <c r="H823" t="s">
+        <v>19</v>
+      </c>
+      <c r="I823">
+        <v>0</v>
+      </c>
+      <c r="J823">
+        <v>15</v>
+      </c>
+      <c r="K823" t="s">
+        <v>19</v>
+      </c>
+      <c r="M823" t="s">
+        <v>2372</v>
+      </c>
+      <c r="N823" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O823">
+        <v>1</v>
+      </c>
+      <c r="P823">
+        <v>1</v>
+      </c>
+      <c r="Q823">
+        <v>0</v>
+      </c>
+      <c r="R823" t="s">
+        <v>20</v>
+      </c>
+      <c r="S823" t="str">
+        <f t="shared" si="33"/>
+        <v>'ROGER_EBERTS_GREAT_MOVIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Roger Eberts Great Movies| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="824" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A824" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B824" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C824">
+        <v>-500</v>
+      </c>
+      <c r="D824">
+        <v>1500</v>
+      </c>
+      <c r="E824">
+        <v>850</v>
+      </c>
+      <c r="F824" t="s">
+        <v>18</v>
+      </c>
+      <c r="H824" t="s">
+        <v>19</v>
+      </c>
+      <c r="I824">
+        <v>0</v>
+      </c>
+      <c r="J824">
+        <v>15</v>
+      </c>
+      <c r="K824" t="s">
+        <v>19</v>
+      </c>
+      <c r="M824" t="s">
+        <v>2364</v>
+      </c>
+      <c r="N824" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O824">
+        <v>1</v>
+      </c>
+      <c r="P824">
+        <v>1</v>
+      </c>
+      <c r="Q824">
+        <v>0</v>
+      </c>
+      <c r="R824" t="s">
+        <v>20</v>
+      </c>
+      <c r="S824" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_250_WOMEN_DIRECTED| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Women-Directed| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="825" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B825" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C825">
+        <v>-500</v>
+      </c>
+      <c r="D825">
+        <v>1500</v>
+      </c>
+      <c r="E825">
+        <v>850</v>
+      </c>
+      <c r="F825" t="s">
+        <v>18</v>
+      </c>
+      <c r="H825" t="s">
+        <v>19</v>
+      </c>
+      <c r="I825">
+        <v>0</v>
+      </c>
+      <c r="J825">
+        <v>15</v>
+      </c>
+      <c r="K825" t="s">
+        <v>19</v>
+      </c>
+      <c r="M825" t="s">
+        <v>2365</v>
+      </c>
+      <c r="N825" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O825">
+        <v>1</v>
+      </c>
+      <c r="P825">
+        <v>1</v>
+      </c>
+      <c r="Q825">
+        <v>0</v>
+      </c>
+      <c r="R825" t="s">
+        <v>20</v>
+      </c>
+      <c r="S825" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_100_BLACK_DIRECTED| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 100 Black-Directed| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="826" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A826" t="s">
+        <v>2352</v>
+      </c>
+      <c r="B826" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C826">
+        <v>-500</v>
+      </c>
+      <c r="D826">
+        <v>1500</v>
+      </c>
+      <c r="E826">
+        <v>850</v>
+      </c>
+      <c r="F826" t="s">
+        <v>18</v>
+      </c>
+      <c r="H826" t="s">
+        <v>19</v>
+      </c>
+      <c r="I826">
+        <v>0</v>
+      </c>
+      <c r="J826">
+        <v>15</v>
+      </c>
+      <c r="K826" t="s">
+        <v>19</v>
+      </c>
+      <c r="M826" t="s">
+        <v>2366</v>
+      </c>
+      <c r="N826" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O826">
+        <v>1</v>
+      </c>
+      <c r="P826">
+        <v>1</v>
+      </c>
+      <c r="Q826">
+        <v>0</v>
+      </c>
+      <c r="R826" t="s">
+        <v>20</v>
+      </c>
+      <c r="S826" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_250_MOST_FANS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Most Fans| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="827" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A827" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B827" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C827">
+        <v>-500</v>
+      </c>
+      <c r="D827">
+        <v>1500</v>
+      </c>
+      <c r="E827">
+        <v>850</v>
+      </c>
+      <c r="F827" t="s">
+        <v>18</v>
+      </c>
+      <c r="H827" t="s">
+        <v>19</v>
+      </c>
+      <c r="I827">
+        <v>0</v>
+      </c>
+      <c r="J827">
+        <v>15</v>
+      </c>
+      <c r="K827" t="s">
+        <v>19</v>
+      </c>
+      <c r="M827" t="s">
+        <v>2367</v>
+      </c>
+      <c r="N827" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O827">
+        <v>1</v>
+      </c>
+      <c r="P827">
+        <v>1</v>
+      </c>
+      <c r="Q827">
+        <v>0</v>
+      </c>
+      <c r="R827" t="s">
+        <v>20</v>
+      </c>
+      <c r="S827" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_250_DOCUMENTARIES| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Documentaries| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="828" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A828" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B828" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C828">
+        <v>-500</v>
+      </c>
+      <c r="D828">
+        <v>1500</v>
+      </c>
+      <c r="E828">
+        <v>850</v>
+      </c>
+      <c r="F828" t="s">
+        <v>18</v>
+      </c>
+      <c r="H828" t="s">
+        <v>19</v>
+      </c>
+      <c r="I828">
+        <v>0</v>
+      </c>
+      <c r="J828">
+        <v>15</v>
+      </c>
+      <c r="K828" t="s">
+        <v>19</v>
+      </c>
+      <c r="M828" t="s">
+        <v>2368</v>
+      </c>
+      <c r="N828" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O828">
+        <v>1</v>
+      </c>
+      <c r="P828">
+        <v>1</v>
+      </c>
+      <c r="Q828">
+        <v>0</v>
+      </c>
+      <c r="R828" t="s">
+        <v>20</v>
+      </c>
+      <c r="S828" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_100_ANIMATION| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 100 Animation| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="829" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A829" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B829" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C829">
+        <v>-500</v>
+      </c>
+      <c r="D829">
+        <v>1500</v>
+      </c>
+      <c r="E829">
+        <v>850</v>
+      </c>
+      <c r="F829" t="s">
+        <v>18</v>
+      </c>
+      <c r="H829" t="s">
+        <v>19</v>
+      </c>
+      <c r="I829">
+        <v>0</v>
+      </c>
+      <c r="J829">
+        <v>15</v>
+      </c>
+      <c r="K829" t="s">
+        <v>19</v>
+      </c>
+      <c r="M829" t="s">
+        <v>2369</v>
+      </c>
+      <c r="N829" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O829">
+        <v>1</v>
+      </c>
+      <c r="P829">
+        <v>1</v>
+      </c>
+      <c r="Q829">
+        <v>0</v>
+      </c>
+      <c r="R829" t="s">
+        <v>20</v>
+      </c>
+      <c r="S829" t="str">
+        <f t="shared" si="33"/>
+        <v>'TOP_250_HORROR| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Top 250 Horror| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="830" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A830" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B830" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C830">
+        <v>-500</v>
+      </c>
+      <c r="D830">
+        <v>1500</v>
+      </c>
+      <c r="E830">
+        <v>850</v>
+      </c>
+      <c r="F830" t="s">
+        <v>18</v>
+      </c>
+      <c r="H830" t="s">
+        <v>19</v>
+      </c>
+      <c r="I830">
+        <v>0</v>
+      </c>
+      <c r="J830">
+        <v>15</v>
+      </c>
+      <c r="K830" t="s">
+        <v>19</v>
+      </c>
+      <c r="M830" t="s">
+        <v>2370</v>
+      </c>
+      <c r="N830" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O830">
+        <v>1</v>
+      </c>
+      <c r="P830">
+        <v>1</v>
+      </c>
+      <c r="Q830">
+        <v>0</v>
+      </c>
+      <c r="R830" t="s">
+        <v>20</v>
+      </c>
+      <c r="S830" t="str">
+        <f t="shared" si="33"/>
+        <v>'IMDB_TOP_250| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | IMDb Top 250| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="831" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A831" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B831" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C831">
+        <v>-500</v>
+      </c>
+      <c r="D831">
+        <v>1500</v>
+      </c>
+      <c r="E831">
+        <v>850</v>
+      </c>
+      <c r="F831" t="s">
+        <v>18</v>
+      </c>
+      <c r="H831" t="s">
+        <v>19</v>
+      </c>
+      <c r="I831">
+        <v>0</v>
+      </c>
+      <c r="J831">
+        <v>15</v>
+      </c>
+      <c r="K831" t="s">
+        <v>19</v>
+      </c>
+      <c r="M831" t="s">
+        <v>2374</v>
+      </c>
+      <c r="N831" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O831">
+        <v>1</v>
+      </c>
+      <c r="P831">
+        <v>1</v>
+      </c>
+      <c r="Q831">
+        <v>0</v>
+      </c>
+      <c r="R831" t="s">
+        <v>20</v>
+      </c>
+      <c r="S831" t="str">
+        <f t="shared" si="33"/>
+        <v>'OSCARS_BEST_PICTURE_WINNERS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Oscars Best Picture Winners| #405162| 1| 1| 0| 0',</v>
+      </c>
+    </row>
+    <row r="832" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A832" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B832" t="s">
+        <v>2359</v>
+      </c>
+      <c r="C832">
+        <v>-500</v>
+      </c>
+      <c r="D832">
+        <v>1500</v>
+      </c>
+      <c r="E832">
+        <v>850</v>
+      </c>
+      <c r="F832" t="s">
+        <v>18</v>
+      </c>
+      <c r="H832" t="s">
+        <v>19</v>
+      </c>
+      <c r="I832">
+        <v>0</v>
+      </c>
+      <c r="J832">
+        <v>15</v>
+      </c>
+      <c r="K832" t="s">
+        <v>19</v>
+      </c>
+      <c r="M832" t="s">
+        <v>2373</v>
+      </c>
+      <c r="N832" t="s">
+        <v>2376</v>
+      </c>
+      <c r="O832">
+        <v>1</v>
+      </c>
+      <c r="P832">
+        <v>1</v>
+      </c>
+      <c r="Q832">
+        <v>0</v>
+      </c>
+      <c r="R832" t="s">
+        <v>20</v>
+      </c>
+      <c r="S832" t="str">
+        <f t="shared" si="33"/>
         <v>'CANNES_PALMES_DOR_WINNERS| Letterboxd.png| +-500| 1500| +850| ComfortAa-Medium| | #FFFFFF| 0| 15| #FFFFFF| | Cannes Palme dOr Winners| #405162| 1| 1| 0| 0',</v>
       </c>
     </row>
@@ -51459,13 +53115,13 @@
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M20 N2:N178">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>